<commit_message>
GUI required completed, layout still weird
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,6 +501,40 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01:04:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01:10:14</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
can save in xls in runtime
</commit_message>
<xml_diff>
--- a/Attendance.xlsx
+++ b/Attendance.xlsx
@@ -8,6 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Attendance" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Attendance1" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Attendance2" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -555,4 +558,486 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>23:12:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23:14:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01:04:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01:10:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20:37:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>21:50:37</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>23:12:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23:14:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01:04:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01:10:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20:37:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>21:56:26</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Timestamp</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>23:12:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>23:13:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2023-04-25</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>23:14:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>01:04:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>01:10:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>owen-4</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20:37:39</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Noom-157</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>21:56:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>owen-64070103</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2023-04-26</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>21:56:30</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>